<commit_message>
updates to name generator
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox (Personal)/masayuki_kishi/repositories/create_names_v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20253AAA-12F3-5D4C-9526-D1901BEC5D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86605750-D86C-9C4C-9785-652091E5EF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29860" windowHeight="17160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="14">
   <si>
     <t>keyword_type_1</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>modifier_2</t>
+  </si>
+  <si>
+    <t>adje</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>no_cut</t>
   </si>
 </sst>
 </file>
@@ -143,14 +152,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -536,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMM37"/>
+  <dimension ref="A1:AMM40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -551,6 +553,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,115 +580,187 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>6</v>
@@ -691,16 +768,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>4</v>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>6</v>
@@ -708,16 +788,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>6</v>
@@ -725,33 +808,48 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>6</v>
@@ -759,16 +857,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>6</v>
@@ -776,16 +883,25 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E17" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F17" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>6</v>
@@ -793,16 +909,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F18" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>6</v>
@@ -810,16 +935,25 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>6</v>
@@ -827,16 +961,25 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E20" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>6</v>
@@ -844,16 +987,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F21" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>6</v>
@@ -861,16 +1013,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>6</v>
@@ -878,16 +1039,25 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C23" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E23" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>6</v>
@@ -895,16 +1065,25 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E24" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>6</v>
@@ -912,16 +1091,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C25" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D25" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>6</v>
@@ -929,16 +1117,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C26" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E26" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F26" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>6</v>
@@ -946,16 +1143,25 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C27" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E27" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F27" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>6</v>
@@ -963,16 +1169,25 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D28" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>6</v>
@@ -980,16 +1195,25 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E29" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F29" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>6</v>
@@ -997,16 +1221,25 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E30" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F30" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>6</v>
@@ -1014,16 +1247,25 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>6</v>
@@ -1031,16 +1273,25 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E32" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F32" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>6</v>
@@ -1048,16 +1299,25 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E33" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F33" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>6</v>
@@ -1065,16 +1325,25 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>6</v>
@@ -1082,16 +1351,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F35" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>6</v>
@@ -1099,16 +1377,25 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E36" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F36" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>6</v>
@@ -1116,18 +1403,96 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H37" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated name generation output
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox (Personal)/masayuki_kishi/repositories/create_names_v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86605750-D86C-9C4C-9785-652091E5EF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9B9683-D813-D94F-8FA4-91D401EF0F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29860" windowHeight="17160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="algorithms" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="15">
   <si>
     <t>keyword_type_1</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>no_cut</t>
+  </si>
+  <si>
+    <t>compent type</t>
   </si>
 </sst>
 </file>
@@ -541,18 +544,19 @@
   <dimension ref="A1:AMM40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5" style="2" customWidth="1"/>
     <col min="2" max="8" width="23" style="2" customWidth="1"/>
-    <col min="9" max="1027" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="37.6640625" style="2" customWidth="1"/>
+    <col min="10" max="1027" width="10.83203125" style="2"/>
     <col min="1028" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -577,8 +581,11 @@
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -593,7 +600,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -607,11 +614,8 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -625,11 +629,8 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -646,7 +647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -662,11 +663,8 @@
       <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -682,11 +680,8 @@
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -702,11 +697,8 @@
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -722,11 +714,8 @@
       <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -742,11 +731,8 @@
       <c r="E10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -762,11 +748,8 @@
       <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -782,11 +765,8 @@
       <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -802,11 +782,8 @@
       <c r="E13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -828,8 +805,11 @@
       <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -855,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1428,6 +1408,9 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
       <c r="B38" s="2" t="s">
         <v>11</v>
       </c>
@@ -1451,6 +1434,9 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
       <c r="B39" s="2" t="s">
         <v>11</v>
       </c>
@@ -1474,6 +1460,9 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
       <c r="B40" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
removed keyword scoring, updated keyword generation, updated name generation
</commit_message>
<xml_diff>
--- a/algorithm_list.xlsx
+++ b/algorithm_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox (Personal)/masayuki_kishi/repositories/create_names_v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9B9683-D813-D94F-8FA4-91D401EF0F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02A5F4D-D1AA-0249-8E7D-81C39ACD8B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="algorithms" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="17">
   <si>
     <t>keyword_type_1</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>compent type</t>
+  </si>
+  <si>
+    <t>pref</t>
+  </si>
+  <si>
+    <t>suff</t>
   </si>
 </sst>
 </file>
@@ -541,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMM40"/>
+  <dimension ref="A1:AMM42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -788,7 +794,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>13</v>
@@ -798,15 +804,6 @@
       </c>
       <c r="E14" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -820,19 +817,10 @@
         <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -846,7 +834,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>13</v>
@@ -872,13 +860,13 @@
         <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>13</v>
@@ -898,13 +886,13 @@
         <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>13</v>
@@ -924,7 +912,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>13</v>
@@ -950,13 +938,13 @@
         <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>13</v>
@@ -976,13 +964,13 @@
         <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>13</v>
@@ -1002,7 +990,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>13</v>
@@ -1022,19 +1010,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>13</v>
@@ -1048,19 +1036,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>13</v>
@@ -1080,7 +1068,7 @@
         <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>13</v>
@@ -1106,13 +1094,13 @@
         <v>13</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>13</v>
@@ -1132,13 +1120,13 @@
         <v>13</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>13</v>
@@ -1158,7 +1146,7 @@
         <v>13</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>13</v>
@@ -1184,13 +1172,13 @@
         <v>13</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>13</v>
@@ -1210,13 +1198,13 @@
         <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>13</v>
@@ -1236,7 +1224,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>13</v>
@@ -1256,19 +1244,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>13</v>
@@ -1282,19 +1270,19 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>13</v>
@@ -1314,7 +1302,7 @@
         <v>13</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>13</v>
@@ -1340,13 +1328,13 @@
         <v>13</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>13</v>
@@ -1366,13 +1354,13 @@
         <v>13</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>13</v>
@@ -1392,7 +1380,7 @@
         <v>13</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>13</v>
@@ -1418,13 +1406,13 @@
         <v>13</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>13</v>
@@ -1444,13 +1432,13 @@
         <v>13</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>13</v>
@@ -1470,7 +1458,7 @@
         <v>13</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>13</v>
@@ -1482,6 +1470,58 @@
         <v>13</v>
       </c>
       <c r="H40" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>